<commit_message>
input field colspan ____ bayar zakat UX
</commit_message>
<xml_diff>
--- a/public/template/PayZakat - Templat Pembayar Zakat.xlsx
+++ b/public/template/PayZakat - Templat Pembayar Zakat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Git\PayZakat\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Git\payzakat\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve"> No Kad Pengenalan Baru</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t xml:space="preserve"> E-mel</t>
+  </si>
+  <si>
+    <t>Nilai Pembayaran Zakat</t>
   </si>
 </sst>
 </file>
@@ -399,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +430,7 @@
     <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -484,6 +487,9 @@
       </c>
       <c r="S1" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>